<commit_message>
Add all test scripts, config, and Excel file
</commit_message>
<xml_diff>
--- a/IT23366718- Test cases (1).xlsx
+++ b/IT23366718- Test cases (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEB06E3-0A55-4E53-B5BF-AB01CDC77B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFCE048-A708-4F07-968F-5E2EB16CFBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="476">
   <si>
     <t>TC ID</t>
   </si>
@@ -6299,6 +6299,10 @@
   </si>
   <si>
     <t>UI preserves formatting in multi-line input</t>
+  </si>
+  <si>
+    <t>mata nidhimathayi.
+dhaen vahinavaa.</t>
   </si>
   <si>
     <t>මට නිදිමතයි.
@@ -7273,7 +7277,7 @@
   <dimension ref="A1:R145"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D130" sqref="D130:D133"/>
+      <selection activeCell="D142" sqref="D142:D145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7460,7 +7464,7 @@
         <v>11</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>257</v>
@@ -7475,7 +7479,7 @@
       <c r="F11" s="28"/>
       <c r="G11" s="24"/>
       <c r="H11" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>258</v>
@@ -7490,7 +7494,7 @@
       <c r="F12" s="28"/>
       <c r="G12" s="24"/>
       <c r="H12" s="21" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>21</v>
@@ -7530,7 +7534,7 @@
         <v>11</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>19</v>
@@ -7545,7 +7549,7 @@
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
       <c r="H15" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>263</v>
@@ -8570,25 +8574,25 @@
         <v>353</v>
       </c>
       <c r="B74" s="24" t="s">
+        <v>457</v>
+      </c>
+      <c r="C74" s="24" t="s">
         <v>456</v>
       </c>
-      <c r="C74" s="24" t="s">
+      <c r="D74" s="26" t="s">
+        <v>449</v>
+      </c>
+      <c r="E74" s="26" t="s">
         <v>455</v>
       </c>
-      <c r="D74" s="26" t="s">
-        <v>448</v>
-      </c>
-      <c r="E74" s="26" t="s">
-        <v>454</v>
-      </c>
       <c r="F74" s="26" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="G74" s="24" t="s">
         <v>11</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="I74" s="2" t="s">
         <v>345</v>
@@ -8603,10 +8607,10 @@
       <c r="F75" s="26"/>
       <c r="G75" s="24"/>
       <c r="H75" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -8619,7 +8623,7 @@
       <c r="G76" s="24"/>
       <c r="H76" s="2"/>
       <c r="I76" s="2" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -8712,13 +8716,13 @@
         <v>10</v>
       </c>
       <c r="D82" s="26" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E82" s="26" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="F82" s="26" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="G82" s="24" t="s">
         <v>11</v>
@@ -8780,7 +8784,7 @@
         <v>10</v>
       </c>
       <c r="D86" s="26" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E86" s="26" t="s">
         <v>362</v>
@@ -8931,7 +8935,7 @@
         <v>374</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -8987,10 +8991,10 @@
         <v>359</v>
       </c>
       <c r="E98" s="26" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="F98" s="26" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G98" s="24" t="s">
         <v>11</v>
@@ -9196,7 +9200,7 @@
         <v>11</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="I110" s="2" t="s">
         <v>395</v>
@@ -9412,28 +9416,28 @@
         <v>410</v>
       </c>
       <c r="B122" s="24" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C122" s="24" t="s">
         <v>16</v>
       </c>
       <c r="D122" s="26" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="E122" s="26" t="s">
+        <v>468</v>
+      </c>
+      <c r="F122" s="26" t="s">
         <v>467</v>
-      </c>
-      <c r="F122" s="26" t="s">
-        <v>466</v>
       </c>
       <c r="G122" s="24" t="s">
         <v>437</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="I122" s="2" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="123" spans="1:18" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -9478,25 +9482,25 @@
         <v>417</v>
       </c>
       <c r="B126" s="24" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C126" s="24" t="s">
         <v>16</v>
       </c>
       <c r="D126" s="26" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="E126" s="26" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F126" s="26" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="G126" s="24" t="s">
         <v>437</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="I126" s="2" t="s">
         <v>356</v>
@@ -9512,7 +9516,7 @@
       <c r="G127" s="24"/>
       <c r="H127" s="2"/>
       <c r="I127" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="128" spans="1:18" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -9643,7 +9647,7 @@
       <c r="F135" s="26"/>
       <c r="G135" s="24"/>
       <c r="H135" s="33" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="I135" s="2" t="s">
         <v>396</v>
@@ -9684,13 +9688,13 @@
         <v>16</v>
       </c>
       <c r="D138" s="26" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E138" s="26" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="F138" s="26" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="G138" s="24" t="s">
         <v>437</v>
@@ -9711,7 +9715,7 @@
       <c r="F139" s="26"/>
       <c r="G139" s="24"/>
       <c r="H139" s="32" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="I139" s="2" t="s">
         <v>436</v>
@@ -9752,19 +9756,19 @@
         <v>16</v>
       </c>
       <c r="D142" s="26" t="s">
-        <v>461</v>
+        <v>439</v>
       </c>
       <c r="E142" s="26" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="F142" s="26" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G142" s="24" t="s">
         <v>11</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I142" s="2" t="s">
         <v>345</v>

</xml_diff>